<commit_message>
SIQ Peer Review Notes Added
Add 2 SIQ rows in SIQ sheet
</commit_message>
<xml_diff>
--- a/SIQ 1.3.xlsx
+++ b/SIQ 1.3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossa\Documents\GitHub\Foodies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dina\Documents\GitHub\Foodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25714" windowHeight="13723"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25716" windowHeight="13728" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="143">
   <si>
     <t>ID</t>
   </si>
@@ -560,6 +560,30 @@
   </si>
   <si>
     <t>Author</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_025</t>
+  </si>
+  <si>
+    <t>if we enter incorrect data or let the field empty what will happen?</t>
+  </si>
+  <si>
+    <t>text message in red color appears next or under the field</t>
+  </si>
+  <si>
+    <t>"Please Enter Valid Data"/Next to Field</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search bar exist in all pages or in specific page </t>
+  </si>
+  <si>
+    <t>in home page only</t>
+  </si>
+  <si>
+    <t>Please add in SIQ sheet</t>
   </si>
 </sst>
 </file>
@@ -1064,21 +1088,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.69140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.69140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="72.53515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.765625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="72.5546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="37" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="8.84375" style="12"/>
+    <col min="6" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="41.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
@@ -1095,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>46</v>
       </c>
@@ -1109,7 +1133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>46</v>
       </c>
@@ -1126,7 +1150,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -1140,7 +1164,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>46</v>
       </c>
@@ -1157,7 +1181,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>86</v>
       </c>
@@ -1174,7 +1198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="14">
         <v>1.3</v>
       </c>
@@ -1188,7 +1212,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="14">
         <v>1.3</v>
       </c>
@@ -1212,24 +1236,24 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.15234375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.15234375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="56.765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.15234375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" style="1"/>
-    <col min="7" max="7" width="23.3046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.69140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.3046875" style="1"/>
+    <col min="1" max="1" width="20.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="37.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="34.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -1263,7 +1287,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>91</v>
       </c>
@@ -1280,7 +1304,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
@@ -1297,7 +1321,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -1314,7 +1338,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>91</v>
       </c>
@@ -1331,7 +1355,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>91</v>
       </c>
@@ -1348,7 +1372,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>91</v>
       </c>
@@ -1365,7 +1389,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>91</v>
       </c>
@@ -1382,7 +1406,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>92</v>
       </c>
@@ -1399,7 +1423,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>92</v>
       </c>
@@ -1416,7 +1440,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>92</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>92</v>
       </c>
@@ -1450,7 +1474,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>92</v>
       </c>
@@ -1467,7 +1491,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>92</v>
       </c>
@@ -1484,7 +1508,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>93</v>
       </c>
@@ -1501,7 +1525,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>94</v>
       </c>
@@ -1518,7 +1542,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>94</v>
       </c>
@@ -1535,7 +1559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>94</v>
       </c>
@@ -1552,7 +1576,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>91</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
@@ -1580,7 +1604,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
@@ -1594,7 +1618,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>91</v>
       </c>
@@ -1608,7 +1632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>92</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
@@ -1636,7 +1660,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
     </row>
@@ -1648,22 +1672,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.3046875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="54.3046875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="59.3828125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="36.53515625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.84375" style="9"/>
+    <col min="1" max="1" width="27.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="41.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1677,7 +1702,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1688,7 +1713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="50.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1699,7 +1724,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="83.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="104.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="66.900000000000006" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1718,7 +1743,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="50.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1729,7 +1754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1737,12 +1762,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1750,7 +1775,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33.450000000000003" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1761,7 +1786,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="33.450000000000003" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>43</v>
       </c>
@@ -1775,7 +1800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1786,7 +1811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="50.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -1797,12 +1822,46 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="11" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="11" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>